<commit_message>
refactored measureDescriptionId to use measure description and sequence to support link from master to description
</commit_message>
<xml_diff>
--- a/ISO19157-3/ISO19157-3_DQM.xlsx
+++ b/ISO19157-3/ISO19157-3_DQM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\272813d\data\standards\ISO\ISO_19157-3\OGC\25sep20_DEMO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\ogc\iso19157-3-dqm-register\ISO19157-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331B2DBD-4E86-47D0-B695-D80F08D6F7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142B1439-D1D1-4F27-A930-C442DF98B268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{07ECC0CD-EFD9-442B-A5D4-A97E92D71BA8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" firstSheet="1" activeTab="4" xr2:uid="{07ECC0CD-EFD9-442B-A5D4-A97E92D71BA8}"/>
   </bookViews>
   <sheets>
     <sheet name="dataQualityMeasures" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="188">
   <si>
     <t>Name</t>
   </si>
@@ -306,9 +306,6 @@
     <t>textDescription</t>
   </si>
   <si>
-    <t>fromulaType ID</t>
-  </si>
-  <si>
     <t>languageVersion</t>
   </si>
   <si>
@@ -348,9 +345,6 @@
     <t>parameter</t>
   </si>
   <si>
-    <t>measureDescriptionID</t>
-  </si>
-  <si>
     <t>language</t>
   </si>
   <si>
@@ -378,22 +372,13 @@
     <t>https://standards.isotc211.org/19157/-3/1/dqc/content/measureDescription/MD49</t>
   </si>
   <si>
-    <t>https://standards.isotc211.org/19157/-3/1/dqc/content/measureDescription/MD28</t>
-  </si>
-  <si>
     <t>0,054 meter</t>
   </si>
   <si>
     <t>The value true indicates that an item is missing.</t>
   </si>
   <si>
-    <t>https://standards.isotc211.org/19157/-3/1/dqc/content/measureDescription/MD5</t>
-  </si>
-  <si>
     <t>https://standards.isotc211.org/19157/-3/1/dqc/basicMeasure/1</t>
-  </si>
-  <si>
-    <t>https://standards.isotc211.org/19157/-3/1/dqc/content/measureDescription/MD5example</t>
   </si>
   <si>
     <t>A data product specification requires all towers higher than 300 m to be captured. The data quality measure “missing item” allows a data quality evaluator or a data user to report that a specific item, in this case a feature of type “tower” (name depends on the application schema), is missing.
@@ -1340,18 +1325,6 @@
       </rPr>
       <t>Y</t>
     </r>
-  </si>
-  <si>
-    <t>https://standards.isotc211.org/19157/-3/1/dqc/content/measureDescription/MD28_1</t>
-  </si>
-  <si>
-    <t>https://standards.isotc211.org/19157/-3/1/dqc/content/measureDescription/MD28_2</t>
-  </si>
-  <si>
-    <t>https://standards.isotc211.org/19157/-3/1/dqc/content/measureDescription/MD28_4</t>
-  </si>
-  <si>
-    <t>https://standards.isotc211.org/19157/-3/1/dqc/content/measureDescription/MD28_3</t>
   </si>
   <si>
     <t>https://standards.isotc211.org/19157/-3/1/dqc/content/formulaType/FT49_1
@@ -1423,14 +1396,6 @@
     <t>https://standards.isotc211.org/19157/-1/1/dqc/content/qualityMeasure/28</t>
   </si>
   <si>
-    <t>https://github.com/i2vana/ISO19157-3/blob/main/img/62.PNG</t>
-  </si>
-  <si>
-    <t>https://github.com/i2vana/ISO19157-3/blob/main/img/4_1.PNG
-https://github.com/i2vana/ISO19157-3/blob/main/img/4_2.PNG
-https://github.com/i2vana/ISO19157-3/blob/main/img/4_3.PNG</t>
-  </si>
-  <si>
     <t>https://standards.isotc211.org/19157/-3/1/dqc/content/measureDescription/MD62</t>
   </si>
   <si>
@@ -1519,6 +1484,23 @@
   </si>
   <si>
     <t>absolute circular error at 90 % significance level of biased data</t>
+  </si>
+  <si>
+    <t>measureID</t>
+  </si>
+  <si>
+    <t>sequence</t>
+  </si>
+  <si>
+    <t>62.PNG</t>
+  </si>
+  <si>
+    <t>4_1.PNG
+4_2.PNG
+4_3.PNG</t>
+  </si>
+  <si>
+    <t>formulaType ID</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1660,11 +1642,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1987,41 +1964,41 @@
       <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="69.109375" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="80.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="80.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="64" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="13" max="14" width="8.7109375"/>
-    <col min="15" max="15" width="86.5703125" customWidth="1"/>
+    <col min="13" max="14" width="8.6640625"/>
+    <col min="15" max="15" width="86.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="45">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="28.8">
       <c r="A1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>8</v>
@@ -2033,7 +2010,7 @@
         <v>11</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>72</v>
@@ -2049,7 +2026,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="178.5" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2065,7 +2042,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
@@ -2092,11 +2069,11 @@
         <v>15</v>
       </c>
       <c r="O2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="120">
-      <c r="A3" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="100.8">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2112,7 +2089,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
@@ -2139,11 +2116,11 @@
         <v>15</v>
       </c>
       <c r="O3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="150">
-      <c r="A4" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="144">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2186,11 +2163,11 @@
         <v>26</v>
       </c>
       <c r="O4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="90">
-      <c r="A5" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="86.4">
+      <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2200,7 +2177,7 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>30</v>
@@ -2233,11 +2210,11 @@
         <v>15</v>
       </c>
       <c r="O5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="90">
-      <c r="A6" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="86.4">
+      <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2247,7 +2224,7 @@
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>36</v>
@@ -2280,11 +2257,11 @@
         <v>40</v>
       </c>
       <c r="O6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="225">
-      <c r="A7" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="187.2">
+      <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2327,11 +2304,11 @@
         <v>15</v>
       </c>
       <c r="O7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="75">
-      <c r="A8" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="72">
+      <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2374,11 +2351,11 @@
         <v>55</v>
       </c>
       <c r="O8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="120">
-      <c r="A9" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="115.2">
+      <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2421,11 +2398,11 @@
         <v>15</v>
       </c>
       <c r="O9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="90">
-      <c r="A10" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="57.6">
+      <c r="A10" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2441,10 +2418,10 @@
         <v>63</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>9</v>
@@ -2463,11 +2440,11 @@
         <v>15</v>
       </c>
       <c r="O10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="90">
-      <c r="A11" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="86.4">
+      <c r="A11" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2510,11 +2487,11 @@
         <v>15</v>
       </c>
       <c r="O11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" ht="105">
-      <c r="A12" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="1" customFormat="1" ht="100.8">
+      <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2557,11 +2534,11 @@
         <v>15</v>
       </c>
       <c r="O12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" ht="60">
-      <c r="A13" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="1" customFormat="1" ht="57.6">
+      <c r="A13" t="s">
         <v>76</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2577,7 +2554,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="G13" s="12"/>
       <c r="L13" s="1">
@@ -2590,15 +2567,15 @@
         <v>55</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="45">
-      <c r="A14" s="17" t="s">
-        <v>193</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="43.2">
+      <c r="A14" t="s">
+        <v>182</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>49</v>
@@ -2607,10 +2584,10 @@
         <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L14" s="1">
         <v>49</v>
@@ -2622,7 +2599,7 @@
         <v>15</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2645,19 +2622,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" customWidth="1"/>
+    <col min="5" max="5" width="33.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2675,9 +2652,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:6" ht="28.8">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>29</v>
@@ -2705,45 +2682,45 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="77.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="77.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="57.6">
+      <c r="A2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="75">
-      <c r="A2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -2751,13 +2728,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -2770,150 +2747,175 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C66609-5758-4067-9188-E18112A71DFE}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D7" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="84.7109375" customWidth="1"/>
-    <col min="2" max="2" width="56.42578125" customWidth="1"/>
-    <col min="3" max="3" width="86.85546875" customWidth="1"/>
-    <col min="4" max="4" width="76.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="73.21875" customWidth="1"/>
+    <col min="5" max="5" width="76.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>183</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="150">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:5" ht="144">
+      <c r="A2" s="6">
+        <v>49</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="100.8">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="105">
-      <c r="A9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="90">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:5" ht="86.4">
+      <c r="A10">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="90">
-      <c r="A11" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://standards.isotc211.org/19157/-3/1/dqc/content/measureDescription/MD49" xr:uid="{D02AA95D-6C4C-408B-BFF4-B543F453AE99}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2922,110 +2924,110 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="78" customWidth="1"/>
-    <col min="2" max="2" width="64.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="64.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.5546875" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="165">
+    </row>
+    <row r="2" spans="1:5" ht="129.6">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="90">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="86.4">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="150">
-      <c r="A4" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="115.2">
+      <c r="A4" t="s">
+        <v>121</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="75">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="72">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.2">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
         <v>54</v>
@@ -3034,15 +3036,15 @@
         <v>75</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -3051,15 +3053,15 @@
         <v>75</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.2">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
         <v>54</v>
@@ -3068,15 +3070,15 @@
         <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="165">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="144">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
         <v>54</v>
@@ -3085,15 +3087,15 @@
         <v>75</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="105">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="86.4">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
         <v>54</v>
@@ -3102,15 +3104,15 @@
         <v>75</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="90">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="86.4">
       <c r="A11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
@@ -3119,15 +3121,15 @@
         <v>75</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="105">
-      <c r="A12" s="15" t="s">
-        <v>151</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="100.8">
+      <c r="A12" t="s">
+        <v>146</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
         <v>54</v>
@@ -3136,15 +3138,15 @@
         <v>75</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="144">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="165">
-      <c r="A13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C13" t="s">
         <v>54</v>
@@ -3153,15 +3155,15 @@
         <v>75</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="225">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="201.6">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C14" t="s">
         <v>54</v>
@@ -3170,15 +3172,15 @@
         <v>75</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="75">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="72">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
         <v>54</v>
@@ -3187,15 +3189,15 @@
         <v>75</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="180">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="172.8">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
         <v>54</v>
@@ -3204,7 +3206,7 @@
         <v>75</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix missing value in FT ID column
</commit_message>
<xml_diff>
--- a/ISO19157-3/ISO19157-3_DQM.xlsx
+++ b/ISO19157-3/ISO19157-3_DQM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\ogc\iso1957-3-dqm-register\ISO19157-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6CA077-440C-4A56-9DA5-71E287897B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C11592C-8722-45AA-8B74-E473B72256B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="960" windowWidth="27150" windowHeight="14040" tabRatio="712" activeTab="5" xr2:uid="{07ECC0CD-EFD9-442B-A5D4-A97E92D71BA8}"/>
+    <workbookView xWindow="675" yWindow="1140" windowWidth="27150" windowHeight="14040" tabRatio="712" firstSheet="1" activeTab="5" xr2:uid="{07ECC0CD-EFD9-442B-A5D4-A97E92D71BA8}"/>
   </bookViews>
   <sheets>
     <sheet name="URI" sheetId="9" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1901" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="778">
   <si>
     <t>Name</t>
   </si>
@@ -5519,7 +5519,7 @@
   <dimension ref="A1:N91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B15" sqref="B15"/>
       <selection pane="bottomLeft" activeCell="G81" sqref="G81"/>
     </sheetView>
@@ -10997,9 +10997,9 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B15" sqref="B15"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11033,15 +11033,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="129">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="255">
       <c r="A2" t="s">
-        <v>594</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
+        <v>763</v>
+      </c>
+      <c r="B2"/>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>767</v>
       </c>
       <c r="D2" t="s">
         <v>49</v>
@@ -11050,18 +11048,16 @@
         <v>68</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="165">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="6" customFormat="1" ht="409.5">
       <c r="A3" t="s">
-        <v>594</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
+        <v>764</v>
+      </c>
+      <c r="B3"/>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>768</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
@@ -11070,18 +11066,18 @@
         <v>68</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="225">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="129">
       <c r="A4" t="s">
         <v>594</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
@@ -11090,18 +11086,18 @@
         <v>68</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="75">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="165">
       <c r="A5" t="s">
         <v>594</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
         <v>49</v>
@@ -11110,18 +11106,18 @@
         <v>68</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>111</v>
+        <v>562</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="203.25" customHeight="1">
       <c r="A6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>575</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
         <v>49</v>
@@ -11130,18 +11126,18 @@
         <v>68</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="151.5">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="75">
       <c r="A7" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>576</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -11150,15 +11146,18 @@
         <v>68</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="126">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="180">
       <c r="A8" t="s">
-        <v>581</v>
+        <v>595</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="D8" t="s">
         <v>49</v>
@@ -11167,15 +11166,18 @@
         <v>68</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="126">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="151.5">
       <c r="A9" t="s">
-        <v>587</v>
+        <v>595</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
@@ -11184,18 +11186,15 @@
         <v>68</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="75">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="126">
       <c r="A10" t="s">
-        <v>596</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
+        <v>581</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="D10" t="s">
         <v>49</v>
@@ -11204,18 +11203,15 @@
         <v>68</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="315">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="126">
       <c r="A11" t="s">
-        <v>596</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
+        <v>587</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>602</v>
+        <v>586</v>
       </c>
       <c r="D11" t="s">
         <v>49</v>
@@ -11224,15 +11220,18 @@
         <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="61.5">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75">
+      <c r="A12" t="s">
+        <v>596</v>
+      </c>
       <c r="B12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="D12" t="s">
         <v>49</v>
@@ -11241,18 +11240,18 @@
         <v>68</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="135">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="315">
       <c r="A13" t="s">
         <v>596</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D13" t="s">
         <v>49</v>
@@ -11261,18 +11260,18 @@
         <v>68</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="120">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="61.5">
       <c r="A14" t="s">
         <v>596</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="D14" t="s">
         <v>49</v>
@@ -11281,18 +11280,18 @@
         <v>68</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="405">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="135">
       <c r="A15" t="s">
         <v>596</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D15" t="s">
         <v>49</v>
@@ -11301,18 +11300,18 @@
         <v>68</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="135">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="120">
       <c r="A16" t="s">
         <v>596</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="D16" t="s">
         <v>49</v>
@@ -11321,18 +11320,18 @@
         <v>68</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="409.5">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="405">
       <c r="A17" t="s">
         <v>596</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D17" t="s">
         <v>49</v>
@@ -11341,18 +11340,18 @@
         <v>68</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="75">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="135">
       <c r="A18" t="s">
         <v>596</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="D18" t="s">
         <v>49</v>
@@ -11361,18 +11360,18 @@
         <v>68</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="375">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="409.5">
       <c r="A19" t="s">
         <v>596</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="D19" t="s">
         <v>49</v>
@@ -11381,15 +11380,18 @@
         <v>68</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="120">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="75">
       <c r="A20" t="s">
-        <v>618</v>
+        <v>596</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D20" t="s">
         <v>49</v>
@@ -11397,19 +11399,19 @@
       <c r="E20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="105">
+      <c r="F20" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="375">
       <c r="A21" t="s">
-        <v>624</v>
+        <v>596</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="D21" t="s">
         <v>49</v>
@@ -11417,19 +11419,16 @@
       <c r="E21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="105">
+      <c r="F21" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="120">
       <c r="A22" t="s">
-        <v>624</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
+        <v>618</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="D22" t="s">
         <v>49</v>
@@ -11438,18 +11437,18 @@
         <v>68</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="90">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="105">
       <c r="A23" t="s">
         <v>624</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="D23" t="s">
         <v>49</v>
@@ -11458,7 +11457,7 @@
         <v>68</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="88.5" customHeight="1">
@@ -11466,10 +11465,10 @@
         <v>624</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>738</v>
+        <v>628</v>
       </c>
       <c r="D24" t="s">
         <v>49</v>
@@ -11478,18 +11477,18 @@
         <v>68</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="75">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="90">
       <c r="A25" t="s">
         <v>624</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D25" t="s">
         <v>49</v>
@@ -11498,18 +11497,18 @@
         <v>68</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="75">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="90">
       <c r="A26" t="s">
         <v>624</v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>634</v>
+        <v>738</v>
       </c>
       <c r="D26" t="s">
         <v>49</v>
@@ -11518,18 +11517,18 @@
         <v>68</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="90">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="75">
       <c r="A27" t="s">
         <v>624</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="D27" t="s">
         <v>49</v>
@@ -11538,18 +11537,18 @@
         <v>68</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="150">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="75">
       <c r="A28" t="s">
         <v>624</v>
       </c>
       <c r="B28">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D28" t="s">
         <v>49</v>
@@ -11558,18 +11557,18 @@
         <v>68</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="105">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="90">
       <c r="A29" t="s">
-        <v>641</v>
+        <v>624</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>626</v>
+        <v>636</v>
       </c>
       <c r="D29" t="s">
         <v>49</v>
@@ -11578,18 +11577,18 @@
         <v>68</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="120">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="150">
       <c r="A30" t="s">
-        <v>641</v>
+        <v>624</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="D30" t="s">
         <v>49</v>
@@ -11598,18 +11597,18 @@
         <v>68</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="90">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="105">
       <c r="A31" t="s">
         <v>641</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>645</v>
+        <v>626</v>
       </c>
       <c r="D31" t="s">
         <v>49</v>
@@ -11618,18 +11617,18 @@
         <v>68</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="75">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="120">
       <c r="A32" t="s">
         <v>641</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D32" t="s">
         <v>49</v>
@@ -11638,18 +11637,18 @@
         <v>68</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="30">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="90">
       <c r="A33" t="s">
         <v>641</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D33" t="s">
         <v>49</v>
@@ -11658,18 +11657,18 @@
         <v>68</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="180">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="75">
       <c r="A34" t="s">
         <v>641</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D34" t="s">
         <v>49</v>
@@ -11678,19 +11677,19 @@
         <v>68</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>745</v>
+        <v>646</v>
       </c>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" ht="105">
+    <row r="35" spans="1:7" ht="30">
       <c r="A35" t="s">
         <v>641</v>
       </c>
       <c r="B35">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D35" t="s">
         <v>49</v>
@@ -11699,18 +11698,18 @@
         <v>68</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="105">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="180">
       <c r="A36" t="s">
         <v>641</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="D36" t="s">
         <v>49</v>
@@ -11719,15 +11718,18 @@
         <v>68</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="180">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="105">
       <c r="A37" t="s">
-        <v>143</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>94</v>
+        <v>641</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>652</v>
       </c>
       <c r="D37" t="s">
         <v>49</v>
@@ -11736,18 +11738,18 @@
         <v>68</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="211.5">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="105">
       <c r="A38" t="s">
-        <v>658</v>
+        <v>641</v>
       </c>
       <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>660</v>
+        <v>8</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>653</v>
       </c>
       <c r="D38" t="s">
         <v>49</v>
@@ -11756,18 +11758,15 @@
         <v>68</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="165">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="180">
       <c r="A39" t="s">
-        <v>658</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
+        <v>143</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>662</v>
+        <v>94</v>
       </c>
       <c r="D39" t="s">
         <v>49</v>
@@ -11776,18 +11775,18 @@
         <v>68</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="240">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="211.5">
       <c r="A40" t="s">
         <v>658</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="D40" t="s">
         <v>49</v>
@@ -11796,7 +11795,7 @@
         <v>68</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="186.75" customHeight="1">
@@ -11804,10 +11803,10 @@
         <v>658</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>737</v>
+        <v>662</v>
       </c>
       <c r="D41" t="s">
         <v>49</v>
@@ -11816,19 +11815,19 @@
         <v>68</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" ht="90">
+    <row r="42" spans="1:7" ht="240">
       <c r="A42" t="s">
         <v>658</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D42" t="s">
         <v>49</v>
@@ -11837,18 +11836,18 @@
         <v>68</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" ht="165">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="6" customFormat="1" ht="240">
       <c r="A43" t="s">
         <v>658</v>
       </c>
-      <c r="B43" s="17">
-        <v>6</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>669</v>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>737</v>
       </c>
       <c r="D43" t="s">
         <v>49</v>
@@ -11856,19 +11855,19 @@
       <c r="E43" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F43" s="16" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="165">
+      <c r="F43" s="7" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="90">
       <c r="A44" t="s">
-        <v>597</v>
+        <v>658</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>95</v>
+        <v>667</v>
       </c>
       <c r="D44" t="s">
         <v>49</v>
@@ -11876,19 +11875,19 @@
       <c r="E44" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="90">
+      <c r="F44" s="7" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="165">
       <c r="A45" t="s">
-        <v>597</v>
-      </c>
-      <c r="B45">
-        <v>2</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>97</v>
+        <v>658</v>
+      </c>
+      <c r="B45" s="17">
+        <v>6</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>669</v>
       </c>
       <c r="D45" t="s">
         <v>49</v>
@@ -11896,19 +11895,19 @@
       <c r="E45" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="150">
+      <c r="F45" s="16" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="165">
       <c r="A46" t="s">
         <v>597</v>
       </c>
       <c r="B46">
-        <v>3</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>99</v>
+        <v>1</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="D46" t="s">
         <v>49</v>
@@ -11916,19 +11915,19 @@
       <c r="E46" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F46" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="75">
+      <c r="F46" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="90">
       <c r="A47" t="s">
         <v>597</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -11936,19 +11935,19 @@
       <c r="E47" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="19" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45">
+      <c r="F47" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="150">
       <c r="A48" t="s">
         <v>597</v>
       </c>
       <c r="B48">
-        <v>5</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>102</v>
+        <v>3</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>99</v>
       </c>
       <c r="D48" t="s">
         <v>49</v>
@@ -11956,19 +11955,19 @@
       <c r="E48" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="165">
+      <c r="F48" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="75">
       <c r="A49" t="s">
         <v>597</v>
       </c>
       <c r="B49">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D49" t="s">
         <v>49</v>
@@ -11976,20 +11975,20 @@
       <c r="E49" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>671</v>
+      <c r="F49" s="19" t="s">
+        <v>100</v>
       </c>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" ht="105">
+    <row r="50" spans="1:7" ht="45">
       <c r="A50" t="s">
         <v>597</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D50" t="s">
         <v>49</v>
@@ -11997,19 +11996,19 @@
       <c r="E50" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F50" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="90">
+      <c r="F50" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="165">
       <c r="A51" t="s">
         <v>597</v>
       </c>
       <c r="B51">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D51" t="s">
         <v>49</v>
@@ -12018,18 +12017,18 @@
         <v>68</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="135">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="105">
       <c r="A52" t="s">
-        <v>675</v>
+        <v>597</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>679</v>
+        <v>105</v>
       </c>
       <c r="D52" t="s">
         <v>49</v>
@@ -12037,19 +12036,19 @@
       <c r="E52" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="210">
+      <c r="F52" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="90">
       <c r="A53" t="s">
-        <v>675</v>
+        <v>597</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>680</v>
+        <v>107</v>
       </c>
       <c r="D53" t="s">
         <v>49</v>
@@ -12058,18 +12057,18 @@
         <v>68</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="210">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="135">
       <c r="A54" t="s">
         <v>675</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D54" t="s">
         <v>49</v>
@@ -12078,18 +12077,18 @@
         <v>68</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="135">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="210">
       <c r="A55" t="s">
-        <v>686</v>
+        <v>675</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D55" t="s">
         <v>49</v>
@@ -12098,18 +12097,18 @@
         <v>68</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="255">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="210">
       <c r="A56" t="s">
-        <v>686</v>
+        <v>675</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>690</v>
+        <v>681</v>
       </c>
       <c r="D56" t="s">
         <v>49</v>
@@ -12118,18 +12117,18 @@
         <v>68</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="240">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="135">
       <c r="A57" t="s">
         <v>686</v>
       </c>
       <c r="B57">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>691</v>
+        <v>679</v>
       </c>
       <c r="D57" t="s">
         <v>49</v>
@@ -12138,18 +12137,18 @@
         <v>68</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="60">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="255">
       <c r="A58" t="s">
-        <v>695</v>
+        <v>686</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="D58" t="s">
         <v>49</v>
@@ -12158,18 +12157,18 @@
         <v>68</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="135">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="240">
       <c r="A59" t="s">
-        <v>695</v>
+        <v>686</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="D59" t="s">
         <v>49</v>
@@ -12178,18 +12177,18 @@
         <v>68</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="240">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="60">
       <c r="A60" t="s">
         <v>695</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D60" t="s">
         <v>49</v>
@@ -12197,19 +12196,19 @@
       <c r="E60" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F60" s="26" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="105">
+      <c r="F60" s="1" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="135">
       <c r="A61" t="s">
         <v>695</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D61" t="s">
         <v>49</v>
@@ -12217,20 +12216,20 @@
       <c r="E61" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F61" s="26" t="s">
-        <v>702</v>
+      <c r="F61" s="1" t="s">
+        <v>698</v>
       </c>
       <c r="G61" s="26"/>
     </row>
-    <row r="62" spans="1:7" ht="60">
+    <row r="62" spans="1:7" ht="240">
       <c r="A62" t="s">
         <v>695</v>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="D62" t="s">
         <v>49</v>
@@ -12238,19 +12237,19 @@
       <c r="E62" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="60">
+      <c r="F62" s="26" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="105">
       <c r="A63" t="s">
-        <v>708</v>
+        <v>695</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>697</v>
+        <v>703</v>
       </c>
       <c r="D63" t="s">
         <v>49</v>
@@ -12258,19 +12257,19 @@
       <c r="E63" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="285">
+      <c r="F63" s="26" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="60">
       <c r="A64" t="s">
-        <v>708</v>
+        <v>695</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="D64" t="s">
         <v>49</v>
@@ -12279,18 +12278,18 @@
         <v>68</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="409.5">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="60">
       <c r="A65" t="s">
         <v>708</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>712</v>
+        <v>697</v>
       </c>
       <c r="D65" t="s">
         <v>49</v>
@@ -12299,18 +12298,18 @@
         <v>68</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="225">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="285">
       <c r="A66" t="s">
         <v>708</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D66" t="s">
         <v>49</v>
@@ -12319,18 +12318,18 @@
         <v>68</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="105">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="409.5">
       <c r="A67" t="s">
         <v>708</v>
       </c>
       <c r="B67">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="D67" t="s">
         <v>49</v>
@@ -12339,18 +12338,18 @@
         <v>68</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="60">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="225">
       <c r="A68" t="s">
         <v>708</v>
       </c>
       <c r="B68">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D68" t="s">
         <v>49</v>
@@ -12359,15 +12358,18 @@
         <v>68</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="409.5">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="105">
       <c r="A69" t="s">
-        <v>492</v>
+        <v>708</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D69" t="s">
         <v>49</v>
@@ -12376,15 +12378,18 @@
         <v>68</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="255">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="60">
       <c r="A70" t="s">
-        <v>763</v>
+        <v>708</v>
+      </c>
+      <c r="B70">
+        <v>6</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>767</v>
+        <v>718</v>
       </c>
       <c r="D70" t="s">
         <v>49</v>
@@ -12393,15 +12398,15 @@
         <v>68</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>765</v>
+        <v>717</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="409.5">
       <c r="A71" t="s">
-        <v>764</v>
+        <v>492</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>768</v>
+        <v>719</v>
       </c>
       <c r="D71" t="s">
         <v>49</v>
@@ -12410,15 +12415,15 @@
         <v>68</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>766</v>
+        <v>721</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F71">
+    <sortCondition ref="A1:A71"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="E44:E48" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -12427,7 +12432,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Params as sub-concepts to hide on main list
</commit_message>
<xml_diff>
--- a/ISO19157-3/ISO19157-3_DQM.xlsx
+++ b/ISO19157-3/ISO19157-3_DQM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\272813d\data\standards\ISO\ISO_19157-3\240924\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\ogc\iso1957-3-dqm-register\ISO19157-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE751DA-1E80-4429-A1B5-93BCD9B2D0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B30CE4F-14A5-4E80-8ACE-B76426BA8312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="712" firstSheet="1" activeTab="1" xr2:uid="{07ECC0CD-EFD9-442B-A5D4-A97E92D71BA8}"/>
+    <workbookView xWindow="1260" yWindow="1020" windowWidth="27150" windowHeight="13995" tabRatio="712" activeTab="7" xr2:uid="{07ECC0CD-EFD9-442B-A5D4-A97E92D71BA8}"/>
   </bookViews>
   <sheets>
     <sheet name="URI" sheetId="9" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2952" uniqueCount="1264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2954" uniqueCount="1266">
   <si>
     <t>number of duplicate feature instances</t>
   </si>
@@ -7751,6 +7751,12 @@
   </si>
   <si>
     <t>BM</t>
+  </si>
+  <si>
+    <t>Param</t>
+  </si>
+  <si>
+    <t>Parameter</t>
   </si>
 </sst>
 </file>
@@ -7948,7 +7954,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8012,17 +8018,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8413,10 +8408,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3172BD-82A1-4B48-B576-8E07319DA0DE}">
   <dimension ref="A1:Q95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B15" sqref="B15"/>
-      <selection pane="bottomLeft" activeCell="M83" sqref="M83"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8538,14 +8533,14 @@
       </c>
       <c r="O2" s="27">
         <f t="shared" ref="O2:O33" ca="1" si="0">NOW()</f>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q2" s="27">
         <f t="shared" ref="Q2:Q65" ca="1" si="1">NOW()</f>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="2" customFormat="1" ht="30">
@@ -8593,14 +8588,14 @@
       </c>
       <c r="O3" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q3" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="2" customFormat="1" ht="45">
@@ -8648,14 +8643,14 @@
       </c>
       <c r="O4" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q4" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="178.5" customHeight="1">
@@ -8703,14 +8698,14 @@
       </c>
       <c r="O5" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q5" s="27">
         <f ca="1">NOW()</f>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="1" customFormat="1" ht="30">
@@ -8758,14 +8753,14 @@
       </c>
       <c r="O6" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q6" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="1" customFormat="1" ht="12.75" customHeight="1">
@@ -8813,14 +8808,14 @@
       </c>
       <c r="O7" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q7" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="46.5" customHeight="1">
@@ -8868,14 +8863,14 @@
       </c>
       <c r="O8" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q8" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="1" customFormat="1" ht="33.6" customHeight="1">
@@ -8923,14 +8918,14 @@
       </c>
       <c r="O9" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q9" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="1" customFormat="1" ht="33.6" customHeight="1">
@@ -8978,14 +8973,14 @@
       </c>
       <c r="O10" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q10" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="1" customFormat="1" ht="45.75" customHeight="1">
@@ -9033,12 +9028,12 @@
       </c>
       <c r="O11" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9086,14 +9081,14 @@
       </c>
       <c r="O12" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q12" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9141,14 +9136,14 @@
       </c>
       <c r="O13" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="Q13" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9196,14 +9191,14 @@
       </c>
       <c r="O14" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q14" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9251,14 +9246,14 @@
       </c>
       <c r="O15" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q15" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9302,14 +9297,14 @@
       </c>
       <c r="O16" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q16" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9357,14 +9352,14 @@
       </c>
       <c r="O17" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q17" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9412,14 +9407,14 @@
       </c>
       <c r="O18" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q18" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="19" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9467,14 +9462,14 @@
       </c>
       <c r="O19" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q19" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="20" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9522,14 +9517,14 @@
       </c>
       <c r="O20" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q20" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="21" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9577,14 +9572,14 @@
       </c>
       <c r="O21" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q21" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="22" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9632,14 +9627,14 @@
       </c>
       <c r="O22" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q22" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="23" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9687,14 +9682,14 @@
       </c>
       <c r="O23" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q23" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="24" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9742,14 +9737,14 @@
       </c>
       <c r="O24" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q24" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="25" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9797,14 +9792,14 @@
       </c>
       <c r="O25" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P25" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q25" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="26" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9852,14 +9847,14 @@
       </c>
       <c r="O26" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P26" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q26" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="27" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9907,14 +9902,14 @@
       </c>
       <c r="O27" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P27" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q27" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="28" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9962,14 +9957,14 @@
       </c>
       <c r="O28" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P28" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q28" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="29" spans="1:17" s="1" customFormat="1" ht="90">
@@ -10009,14 +10004,14 @@
       </c>
       <c r="O29" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P29" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q29" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="30" spans="1:17" s="1" customFormat="1" ht="90">
@@ -10064,14 +10059,14 @@
       </c>
       <c r="O30" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P30" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q30" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="31" spans="1:17" s="5" customFormat="1" ht="90">
@@ -10119,14 +10114,14 @@
       </c>
       <c r="O31" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P31" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q31" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="32" spans="1:17" s="1" customFormat="1" ht="120">
@@ -10174,14 +10169,14 @@
       </c>
       <c r="O32" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P32" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q32" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="33" spans="1:17" s="1" customFormat="1" ht="60">
@@ -10229,14 +10224,14 @@
       </c>
       <c r="O33" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P33" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q33" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="34" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10284,14 +10279,14 @@
       </c>
       <c r="O34" s="27">
         <f t="shared" ref="O34:O65" ca="1" si="2">NOW()</f>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P34" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q34" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10339,14 +10334,14 @@
       </c>
       <c r="O35" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P35" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q35" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="36" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10394,14 +10389,14 @@
       </c>
       <c r="O36" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P36" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q36" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10449,14 +10444,14 @@
       </c>
       <c r="O37" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P37" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q37" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10504,14 +10499,14 @@
       </c>
       <c r="O38" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P38" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q38" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10557,14 +10552,14 @@
       </c>
       <c r="O39" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P39" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q39" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="40" spans="1:17" s="1" customFormat="1" ht="30">
@@ -10612,14 +10607,14 @@
       </c>
       <c r="O40" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P40" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q40" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="41" spans="1:17" s="1" customFormat="1" ht="75">
@@ -10667,14 +10662,14 @@
       </c>
       <c r="O41" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P41" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q41" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="5" customFormat="1" ht="75">
@@ -10719,14 +10714,14 @@
       </c>
       <c r="O42" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P42" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q42" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="43" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10774,14 +10769,14 @@
       </c>
       <c r="O43" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q43" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="44" spans="1:17" s="1" customFormat="1" ht="45">
@@ -10829,14 +10824,14 @@
       </c>
       <c r="O44" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P44" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q44" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="45" spans="1:17" s="1" customFormat="1" ht="75">
@@ -10884,14 +10879,14 @@
       </c>
       <c r="O45" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P45" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q45" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="46" spans="1:17" s="1" customFormat="1" ht="45">
@@ -10939,14 +10934,14 @@
       </c>
       <c r="O46" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P46" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q46" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="47" spans="1:17" s="1" customFormat="1" ht="45">
@@ -10994,14 +10989,14 @@
       </c>
       <c r="O47" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q47" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="48" spans="1:17" s="1" customFormat="1" ht="30">
@@ -11049,14 +11044,14 @@
       </c>
       <c r="O48" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q48" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="49" spans="1:17" s="5" customFormat="1" ht="60">
@@ -11104,14 +11099,14 @@
       </c>
       <c r="O49" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q49" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="50" spans="1:17" s="1" customFormat="1" ht="60">
@@ -11157,14 +11152,14 @@
       </c>
       <c r="O50" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q50" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="51" spans="1:17" s="5" customFormat="1" ht="60">
@@ -11212,14 +11207,14 @@
       </c>
       <c r="O51" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P51" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q51" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="52" spans="1:17" s="5" customFormat="1" ht="60">
@@ -11267,14 +11262,14 @@
       </c>
       <c r="O52" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q52" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="53" spans="1:17" s="1" customFormat="1" ht="90">
@@ -11322,14 +11317,14 @@
       </c>
       <c r="O53" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q53" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="54" spans="1:17" s="1" customFormat="1" ht="60">
@@ -11377,14 +11372,14 @@
       </c>
       <c r="O54" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q54" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="55" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11432,14 +11427,14 @@
       </c>
       <c r="O55" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q55" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="56" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11487,14 +11482,14 @@
       </c>
       <c r="O56" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P56" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q56" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="57" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11542,14 +11537,14 @@
       </c>
       <c r="O57" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P57" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q57" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="58" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11597,14 +11592,14 @@
       </c>
       <c r="O58" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P58" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q58" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="59" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11652,14 +11647,14 @@
       </c>
       <c r="O59" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P59" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q59" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="60" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11707,14 +11702,14 @@
       </c>
       <c r="O60" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P60" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q60" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="61" spans="1:17" s="1" customFormat="1" ht="30">
@@ -11762,14 +11757,14 @@
       </c>
       <c r="O61" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P61" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q61" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="1" customFormat="1" ht="45">
@@ -11817,14 +11812,14 @@
       </c>
       <c r="O62" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P62" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q62" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="63" spans="1:17" s="1" customFormat="1" ht="30">
@@ -11870,14 +11865,14 @@
       </c>
       <c r="O63" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P63" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q63" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="64" spans="1:17" s="1" customFormat="1" ht="45">
@@ -11925,14 +11920,14 @@
       </c>
       <c r="O64" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P64" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q64" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="65" spans="1:17" s="5" customFormat="1" ht="45">
@@ -11980,11 +11975,11 @@
       </c>
       <c r="O65" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="Q65" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="66" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12032,14 +12027,14 @@
       </c>
       <c r="O66" s="27">
         <f t="shared" ref="O66:O95" ca="1" si="3">NOW()</f>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P66" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q66" s="27">
         <f t="shared" ref="Q66:Q95" ca="1" si="4">NOW()</f>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="67" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12087,14 +12082,14 @@
       </c>
       <c r="O67" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P67" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q67" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="68" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12142,14 +12137,14 @@
       </c>
       <c r="O68" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q68" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12197,14 +12192,14 @@
       </c>
       <c r="O69" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q69" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12252,14 +12247,14 @@
       </c>
       <c r="O70" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q70" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="71" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12307,14 +12302,14 @@
       </c>
       <c r="O71" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q71" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="72" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12362,14 +12357,14 @@
       </c>
       <c r="O72" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q72" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12417,14 +12412,14 @@
       </c>
       <c r="O73" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q73" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12472,14 +12467,14 @@
       </c>
       <c r="O74" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P74" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q74" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12527,14 +12522,14 @@
       </c>
       <c r="O75" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P75" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q75" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="76" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12582,14 +12577,14 @@
       </c>
       <c r="O76" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P76" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q76" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="77" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12637,14 +12632,14 @@
       </c>
       <c r="O77" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P77" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q77" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="78" spans="1:17" s="1" customFormat="1" ht="75">
@@ -12692,14 +12687,14 @@
       </c>
       <c r="O78" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P78" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q78" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="79" spans="1:17" s="1" customFormat="1" ht="75">
@@ -12747,14 +12742,14 @@
       </c>
       <c r="O79" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P79" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q79" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="30">
@@ -12802,14 +12797,14 @@
       </c>
       <c r="O80" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P80" s="5" t="s">
         <v>19</v>
       </c>
       <c r="Q80" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="75">
@@ -12857,14 +12852,14 @@
       </c>
       <c r="O81" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P81" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q81" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="30">
@@ -12912,14 +12907,14 @@
       </c>
       <c r="O82" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P82" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q82" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="60">
@@ -12963,14 +12958,14 @@
       </c>
       <c r="O83" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P83" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q83" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="84" spans="1:17" ht="45">
@@ -13018,14 +13013,14 @@
       </c>
       <c r="O84" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P84" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q84" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="45">
@@ -13073,14 +13068,14 @@
       </c>
       <c r="O85" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P85" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q85" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="86" spans="1:17" ht="60">
@@ -13128,14 +13123,14 @@
       </c>
       <c r="O86" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P86" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q86" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="60">
@@ -13183,14 +13178,14 @@
       </c>
       <c r="O87" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P87" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q87" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="30">
@@ -13238,69 +13233,69 @@
       </c>
       <c r="O88" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P88" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q88" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" s="31" customFormat="1" ht="30">
-      <c r="A89" s="30">
+        <v>45560.60788275463</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" ht="30">
+      <c r="A89" s="5">
         <v>207</v>
       </c>
-      <c r="B89" s="30" t="s">
+      <c r="B89" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="C89" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D89" s="30" t="s">
+      <c r="C89" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="E89" s="30" t="s">
+      <c r="E89" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="F89" s="30" t="s">
+      <c r="F89" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="G89" s="30" t="s">
+      <c r="G89" s="5" t="s">
         <v>1043</v>
       </c>
-      <c r="H89" s="32" t="s">
+      <c r="H89" s="12" t="s">
         <v>832</v>
       </c>
-      <c r="I89" s="30" t="s">
+      <c r="I89" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="J89" s="32" t="s">
+      <c r="J89" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K89" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="L89" s="30" t="s">
+      <c r="K89" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L89" s="5" t="s">
         <v>1042</v>
       </c>
-      <c r="M89" s="30" t="s">
+      <c r="M89" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="N89" s="30" t="s">
+      <c r="N89" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="O89" s="33">
+      <c r="O89" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
-      </c>
-      <c r="P89" s="30" t="s">
+        <v>45560.60788275463</v>
+      </c>
+      <c r="P89" s="5" t="s">
         <v>752</v>
       </c>
-      <c r="Q89" s="33">
+      <c r="Q89" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="90" spans="1:17" ht="30">
@@ -13348,14 +13343,14 @@
       </c>
       <c r="O90" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P90" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q90" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="30">
@@ -13403,14 +13398,14 @@
       </c>
       <c r="O91" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q91" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="92" spans="1:17" ht="45">
@@ -13456,14 +13451,14 @@
       </c>
       <c r="O92" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q92" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="30">
@@ -13511,14 +13506,14 @@
       </c>
       <c r="O93" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P93" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q93" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="45">
@@ -13562,14 +13557,14 @@
       </c>
       <c r="O94" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P94" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q94" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="30">
@@ -13615,14 +13610,14 @@
       </c>
       <c r="O95" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
       <c r="P95" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q95" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45559.58315416667</v>
+        <v>45560.60788275463</v>
       </c>
     </row>
   </sheetData>
@@ -16713,25 +16708,25 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="31" customFormat="1">
-      <c r="A112" s="29" t="s">
+    <row r="112" spans="1:5">
+      <c r="A112" s="8" t="s">
         <v>832</v>
       </c>
-      <c r="B112" s="29"/>
-      <c r="C112" s="29"/>
-      <c r="D112" s="29"/>
-      <c r="E112" s="30" t="s">
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="5" t="s">
         <v>1115</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="31" customFormat="1" ht="30">
-      <c r="A113" s="29" t="s">
+    <row r="113" spans="1:5" ht="30">
+      <c r="A113" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="B113" s="29"/>
-      <c r="C113" s="29"/>
-      <c r="D113" s="29"/>
-      <c r="E113" s="30" t="s">
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
+      <c r="E113" s="5" t="s">
         <v>338</v>
       </c>
     </row>
@@ -20301,10 +20296,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099B6858-2052-4C2F-91E5-028849CAB7F9}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20377,6 +20372,14 @@
         <v>85</v>
       </c>
     </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1265</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix missing description and formula reference
</commit_message>
<xml_diff>
--- a/ISO19157-3/ISO19157-3_DQM.xlsx
+++ b/ISO19157-3/ISO19157-3_DQM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\ogc\iso1957-3-dqm-register\ISO19157-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B30CE4F-14A5-4E80-8ACE-B76426BA8312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E883CF-55E9-48BE-848B-F35B1E4F77BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1020" windowWidth="27150" windowHeight="13995" tabRatio="712" activeTab="7" xr2:uid="{07ECC0CD-EFD9-442B-A5D4-A97E92D71BA8}"/>
+    <workbookView xWindow="1260" yWindow="1020" windowWidth="27150" windowHeight="13995" tabRatio="712" activeTab="4" xr2:uid="{07ECC0CD-EFD9-442B-A5D4-A97E92D71BA8}"/>
   </bookViews>
   <sheets>
     <sheet name="URI" sheetId="9" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2954" uniqueCount="1266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="1267">
   <si>
     <t>number of duplicate feature instances</t>
   </si>
@@ -7757,6 +7757,9 @@
   </si>
   <si>
     <t>Parameter</t>
+  </si>
+  <si>
+    <t>FT28_4</t>
   </si>
 </sst>
 </file>
@@ -8409,7 +8412,7 @@
   <dimension ref="A1:Q95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B15" sqref="B15"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
@@ -8510,9 +8513,7 @@
       <c r="G2" s="5" t="s">
         <v>939</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>119</v>
-      </c>
+      <c r="H2" s="12"/>
       <c r="I2" s="20" t="s">
         <v>1</v>
       </c>
@@ -8533,14 +8534,14 @@
       </c>
       <c r="O2" s="27">
         <f t="shared" ref="O2:O33" ca="1" si="0">NOW()</f>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q2" s="27">
         <f t="shared" ref="Q2:Q65" ca="1" si="1">NOW()</f>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="2" customFormat="1" ht="30">
@@ -8588,14 +8589,14 @@
       </c>
       <c r="O3" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q3" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="2" customFormat="1" ht="45">
@@ -8643,14 +8644,14 @@
       </c>
       <c r="O4" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q4" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="178.5" customHeight="1">
@@ -8698,14 +8699,14 @@
       </c>
       <c r="O5" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q5" s="27">
         <f ca="1">NOW()</f>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="1" customFormat="1" ht="30">
@@ -8753,14 +8754,14 @@
       </c>
       <c r="O6" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q6" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="1" customFormat="1" ht="12.75" customHeight="1">
@@ -8808,14 +8809,14 @@
       </c>
       <c r="O7" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q7" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="46.5" customHeight="1">
@@ -8863,14 +8864,14 @@
       </c>
       <c r="O8" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q8" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="1" customFormat="1" ht="33.6" customHeight="1">
@@ -8918,14 +8919,14 @@
       </c>
       <c r="O9" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q9" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="1" customFormat="1" ht="33.6" customHeight="1">
@@ -8973,14 +8974,14 @@
       </c>
       <c r="O10" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q10" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="1" customFormat="1" ht="45.75" customHeight="1">
@@ -9028,12 +9029,12 @@
       </c>
       <c r="O11" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9081,14 +9082,14 @@
       </c>
       <c r="O12" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q12" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9136,14 +9137,14 @@
       </c>
       <c r="O13" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="Q13" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9191,14 +9192,14 @@
       </c>
       <c r="O14" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q14" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9246,14 +9247,14 @@
       </c>
       <c r="O15" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q15" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9297,14 +9298,14 @@
       </c>
       <c r="O16" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q16" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9352,14 +9353,14 @@
       </c>
       <c r="O17" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q17" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9407,14 +9408,14 @@
       </c>
       <c r="O18" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q18" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="19" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9462,14 +9463,14 @@
       </c>
       <c r="O19" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q19" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="20" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9517,14 +9518,14 @@
       </c>
       <c r="O20" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q20" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="21" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9572,14 +9573,14 @@
       </c>
       <c r="O21" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q21" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="22" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9627,14 +9628,14 @@
       </c>
       <c r="O22" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q22" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="23" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9682,14 +9683,14 @@
       </c>
       <c r="O23" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q23" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="24" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9737,14 +9738,14 @@
       </c>
       <c r="O24" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q24" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="25" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9792,14 +9793,14 @@
       </c>
       <c r="O25" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P25" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q25" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="26" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9847,14 +9848,14 @@
       </c>
       <c r="O26" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P26" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q26" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="27" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9902,14 +9903,14 @@
       </c>
       <c r="O27" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P27" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q27" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="28" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9957,14 +9958,14 @@
       </c>
       <c r="O28" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P28" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q28" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="29" spans="1:17" s="1" customFormat="1" ht="90">
@@ -10004,14 +10005,14 @@
       </c>
       <c r="O29" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P29" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q29" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="30" spans="1:17" s="1" customFormat="1" ht="90">
@@ -10059,14 +10060,14 @@
       </c>
       <c r="O30" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P30" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q30" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="31" spans="1:17" s="5" customFormat="1" ht="90">
@@ -10114,14 +10115,14 @@
       </c>
       <c r="O31" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P31" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q31" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="32" spans="1:17" s="1" customFormat="1" ht="120">
@@ -10169,14 +10170,14 @@
       </c>
       <c r="O32" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P32" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q32" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="33" spans="1:17" s="1" customFormat="1" ht="60">
@@ -10224,14 +10225,14 @@
       </c>
       <c r="O33" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P33" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q33" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="34" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10279,14 +10280,14 @@
       </c>
       <c r="O34" s="27">
         <f t="shared" ref="O34:O65" ca="1" si="2">NOW()</f>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P34" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q34" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10334,14 +10335,14 @@
       </c>
       <c r="O35" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P35" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q35" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="36" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10389,14 +10390,14 @@
       </c>
       <c r="O36" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P36" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q36" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10444,14 +10445,14 @@
       </c>
       <c r="O37" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P37" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q37" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10499,14 +10500,14 @@
       </c>
       <c r="O38" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P38" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q38" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10552,14 +10553,14 @@
       </c>
       <c r="O39" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P39" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q39" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="40" spans="1:17" s="1" customFormat="1" ht="30">
@@ -10607,14 +10608,14 @@
       </c>
       <c r="O40" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P40" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q40" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="41" spans="1:17" s="1" customFormat="1" ht="75">
@@ -10662,14 +10663,14 @@
       </c>
       <c r="O41" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P41" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q41" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="5" customFormat="1" ht="75">
@@ -10714,14 +10715,14 @@
       </c>
       <c r="O42" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P42" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q42" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="43" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10769,14 +10770,14 @@
       </c>
       <c r="O43" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q43" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="44" spans="1:17" s="1" customFormat="1" ht="45">
@@ -10824,14 +10825,14 @@
       </c>
       <c r="O44" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P44" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q44" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="45" spans="1:17" s="1" customFormat="1" ht="75">
@@ -10879,14 +10880,14 @@
       </c>
       <c r="O45" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P45" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q45" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="46" spans="1:17" s="1" customFormat="1" ht="45">
@@ -10934,14 +10935,14 @@
       </c>
       <c r="O46" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P46" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q46" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="47" spans="1:17" s="1" customFormat="1" ht="45">
@@ -10989,14 +10990,14 @@
       </c>
       <c r="O47" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q47" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="48" spans="1:17" s="1" customFormat="1" ht="30">
@@ -11044,14 +11045,14 @@
       </c>
       <c r="O48" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q48" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="49" spans="1:17" s="5" customFormat="1" ht="60">
@@ -11099,14 +11100,14 @@
       </c>
       <c r="O49" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q49" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="50" spans="1:17" s="1" customFormat="1" ht="60">
@@ -11152,14 +11153,14 @@
       </c>
       <c r="O50" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q50" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="51" spans="1:17" s="5" customFormat="1" ht="60">
@@ -11207,14 +11208,14 @@
       </c>
       <c r="O51" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P51" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q51" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="52" spans="1:17" s="5" customFormat="1" ht="60">
@@ -11262,14 +11263,14 @@
       </c>
       <c r="O52" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q52" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="53" spans="1:17" s="1" customFormat="1" ht="90">
@@ -11317,14 +11318,14 @@
       </c>
       <c r="O53" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q53" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="54" spans="1:17" s="1" customFormat="1" ht="60">
@@ -11372,14 +11373,14 @@
       </c>
       <c r="O54" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q54" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="55" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11427,14 +11428,14 @@
       </c>
       <c r="O55" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q55" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="56" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11482,14 +11483,14 @@
       </c>
       <c r="O56" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P56" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q56" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="57" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11537,14 +11538,14 @@
       </c>
       <c r="O57" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P57" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q57" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="58" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11592,14 +11593,14 @@
       </c>
       <c r="O58" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P58" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q58" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="59" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11647,14 +11648,14 @@
       </c>
       <c r="O59" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P59" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q59" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="60" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11702,14 +11703,14 @@
       </c>
       <c r="O60" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P60" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q60" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="61" spans="1:17" s="1" customFormat="1" ht="30">
@@ -11757,14 +11758,14 @@
       </c>
       <c r="O61" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P61" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q61" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="1" customFormat="1" ht="45">
@@ -11812,14 +11813,14 @@
       </c>
       <c r="O62" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P62" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q62" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="63" spans="1:17" s="1" customFormat="1" ht="30">
@@ -11865,14 +11866,14 @@
       </c>
       <c r="O63" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P63" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q63" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="64" spans="1:17" s="1" customFormat="1" ht="45">
@@ -11920,14 +11921,14 @@
       </c>
       <c r="O64" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P64" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q64" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="65" spans="1:17" s="5" customFormat="1" ht="45">
@@ -11975,11 +11976,11 @@
       </c>
       <c r="O65" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="Q65" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="66" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12027,14 +12028,14 @@
       </c>
       <c r="O66" s="27">
         <f t="shared" ref="O66:O95" ca="1" si="3">NOW()</f>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P66" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q66" s="27">
         <f t="shared" ref="Q66:Q95" ca="1" si="4">NOW()</f>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="67" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12082,14 +12083,14 @@
       </c>
       <c r="O67" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P67" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q67" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="68" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12137,14 +12138,14 @@
       </c>
       <c r="O68" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q68" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12192,14 +12193,14 @@
       </c>
       <c r="O69" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q69" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12247,14 +12248,14 @@
       </c>
       <c r="O70" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q70" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="71" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12302,14 +12303,14 @@
       </c>
       <c r="O71" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q71" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="72" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12357,14 +12358,14 @@
       </c>
       <c r="O72" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q72" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12412,14 +12413,14 @@
       </c>
       <c r="O73" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q73" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12467,14 +12468,14 @@
       </c>
       <c r="O74" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P74" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q74" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12522,14 +12523,14 @@
       </c>
       <c r="O75" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P75" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q75" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="76" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12577,14 +12578,14 @@
       </c>
       <c r="O76" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P76" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q76" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="77" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12632,14 +12633,14 @@
       </c>
       <c r="O77" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P77" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q77" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="78" spans="1:17" s="1" customFormat="1" ht="75">
@@ -12687,14 +12688,14 @@
       </c>
       <c r="O78" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P78" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q78" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="79" spans="1:17" s="1" customFormat="1" ht="75">
@@ -12742,14 +12743,14 @@
       </c>
       <c r="O79" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P79" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q79" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="30">
@@ -12797,14 +12798,14 @@
       </c>
       <c r="O80" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P80" s="5" t="s">
         <v>19</v>
       </c>
       <c r="Q80" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="75">
@@ -12852,14 +12853,14 @@
       </c>
       <c r="O81" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P81" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q81" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="30">
@@ -12907,14 +12908,14 @@
       </c>
       <c r="O82" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P82" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q82" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="60">
@@ -12958,14 +12959,14 @@
       </c>
       <c r="O83" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P83" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q83" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="84" spans="1:17" ht="45">
@@ -13013,14 +13014,14 @@
       </c>
       <c r="O84" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P84" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q84" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="45">
@@ -13068,14 +13069,14 @@
       </c>
       <c r="O85" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P85" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q85" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="86" spans="1:17" ht="60">
@@ -13123,14 +13124,14 @@
       </c>
       <c r="O86" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P86" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q86" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="60">
@@ -13178,14 +13179,14 @@
       </c>
       <c r="O87" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P87" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q87" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="30">
@@ -13233,14 +13234,14 @@
       </c>
       <c r="O88" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P88" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q88" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="89" spans="1:17" ht="30">
@@ -13288,14 +13289,14 @@
       </c>
       <c r="O89" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P89" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q89" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="90" spans="1:17" ht="30">
@@ -13343,14 +13344,14 @@
       </c>
       <c r="O90" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P90" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q90" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="30">
@@ -13398,14 +13399,14 @@
       </c>
       <c r="O91" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q91" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="92" spans="1:17" ht="45">
@@ -13451,14 +13452,14 @@
       </c>
       <c r="O92" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q92" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="30">
@@ -13506,14 +13507,14 @@
       </c>
       <c r="O93" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P93" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q93" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="45">
@@ -13557,14 +13558,14 @@
       </c>
       <c r="O94" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P94" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q94" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="30">
@@ -13610,14 +13611,14 @@
       </c>
       <c r="O95" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
       <c r="P95" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q95" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45560.60788275463</v>
+        <v>45561.47881458333</v>
       </c>
     </row>
   </sheetData>
@@ -15332,12 +15333,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C66609-5758-4067-9188-E18112A71DFE}">
-  <dimension ref="A1:F189"/>
+  <dimension ref="A1:F190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B15" sqref="B15"/>
-      <selection pane="bottomLeft" activeCell="A112" sqref="A112:XFD113"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16027,115 +16028,115 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" ht="51">
       <c r="A58" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="8">
+        <v>4</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E58" s="5" t="s">
+      <c r="B59" s="8"/>
+      <c r="C59" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>1099</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="18">
-      <c r="A59" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="B59" s="8">
-        <v>1</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="18">
       <c r="A60" s="8" t="s">
         <v>352</v>
       </c>
       <c r="B60" s="8">
+        <v>1</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="45">
+      <c r="A61" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="B61" s="8">
         <v>2</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="63">
-      <c r="A61" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>843</v>
+        <v>357</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="63">
       <c r="A62" s="8" t="s">
-        <v>239</v>
+        <v>359</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" ht="63">
       <c r="A63" s="8" t="s">
         <v>239</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
+      <c r="D63" s="8" t="s">
+        <v>363</v>
+      </c>
       <c r="E63" s="5" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="5" t="s">
         <v>1100</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="60">
-      <c r="A64" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="B64" s="8">
-        <v>1</v>
-      </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="30">
+    <row r="65" spans="1:6" ht="60">
       <c r="A65" s="8" t="s">
         <v>365</v>
       </c>
       <c r="B65" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>374</v>
@@ -16146,11 +16147,11 @@
         <v>365</v>
       </c>
       <c r="B66" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>374</v>
@@ -16161,187 +16162,190 @@
         <v>365</v>
       </c>
       <c r="B67" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" ht="30">
       <c r="A68" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="B68" s="8"/>
+        <v>365</v>
+      </c>
+      <c r="B68" s="8">
+        <v>4</v>
+      </c>
       <c r="C68" s="8"/>
       <c r="D68" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E69" s="5" t="s">
         <v>844</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="120">
-      <c r="A69" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="B69" s="4"/>
-      <c r="C69" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="E69" s="19" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="120">
       <c r="A70" s="8" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="E70" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" ht="120">
       <c r="A71" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
+        <v>401</v>
+      </c>
+      <c r="B71" s="4"/>
+      <c r="C71" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>402</v>
+      </c>
       <c r="E71" s="19" t="s">
-        <v>1161</v>
-      </c>
-      <c r="F71" s="14"/>
+        <v>389</v>
+      </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="8" t="s">
-        <v>415</v>
+        <v>215</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="8"/>
+      <c r="E72" s="19" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F72" s="14"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E72" s="19" t="s">
+      <c r="E73" s="19" t="s">
         <v>1162</v>
       </c>
-      <c r="F72" s="14"/>
-    </row>
-    <row r="73" spans="1:6" ht="90">
-      <c r="A73" s="8" t="s">
+      <c r="F73" s="14"/>
+    </row>
+    <row r="74" spans="1:6" ht="90">
+      <c r="A74" s="8" t="s">
         <v>417</v>
-      </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="120">
-      <c r="A74" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:6" ht="45">
+    </row>
+    <row r="75" spans="1:6" ht="120">
       <c r="A75" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B75" s="4"/>
+      <c r="C75" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" spans="1:6" ht="45">
+      <c r="A76" s="8" t="s">
         <v>430</v>
-      </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="5" t="s">
-        <v>431</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:6" ht="135">
-      <c r="A76" s="8" t="s">
-        <v>441</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="5" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:6" ht="75">
+    <row r="77" spans="1:6" ht="135">
       <c r="A77" s="8" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="5" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:6" ht="90">
+    <row r="78" spans="1:6" ht="75">
       <c r="A78" s="8" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="5" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>451</v>
       </c>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6" ht="30">
+    <row r="79" spans="1:6" ht="90">
       <c r="A79" s="8" t="s">
-        <v>815</v>
+        <v>464</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="5"/>
+      <c r="D79" s="5" t="s">
+        <v>465</v>
+      </c>
       <c r="E79" s="5" t="s">
-        <v>840</v>
+        <v>451</v>
       </c>
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" ht="30">
       <c r="A80" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
@@ -16351,105 +16355,106 @@
       </c>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="1:5" ht="75">
+    <row r="81" spans="1:6" ht="30">
       <c r="A81" s="8" t="s">
+        <v>816</v>
+      </c>
+      <c r="B81" s="4"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5" t="s">
+        <v>840</v>
+      </c>
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" spans="1:6" ht="75">
+      <c r="A82" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="B81" s="8"/>
-      <c r="C81" s="8" t="s">
-        <v>1256</v>
-      </c>
-      <c r="D81" s="8"/>
-      <c r="E81" s="5" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="8" t="s">
-        <v>273</v>
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="8" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="5" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="45">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
+      <c r="C83" s="8" t="s">
+        <v>1257</v>
+      </c>
       <c r="D83" s="8"/>
       <c r="E83" s="5" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="45">
       <c r="A84" s="8" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B84" s="8"/>
-      <c r="C84" s="8" t="s">
-        <v>1258</v>
-      </c>
+      <c r="C84" s="8"/>
       <c r="D84" s="8"/>
       <c r="E84" s="5" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D85" s="8"/>
+      <c r="E85" s="5" t="s">
         <v>1164</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="8" t="s">
+    <row r="86" spans="1:6">
+      <c r="A86" s="8" t="s">
         <v>284</v>
-      </c>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="8" t="s">
-        <v>285</v>
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
+      <c r="D86" s="8" t="s">
+        <v>324</v>
+      </c>
       <c r="E86" s="5" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
       <c r="E87" s="5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" s="8" t="s">
-        <v>817</v>
+        <v>288</v>
       </c>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
       <c r="E88" s="5" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" s="8" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
@@ -16458,31 +16463,31 @@
         <v>841</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:6">
       <c r="A90" s="8" t="s">
-        <v>339</v>
+        <v>818</v>
       </c>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
       <c r="E90" s="5" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" s="8" t="s">
-        <v>819</v>
+        <v>339</v>
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
       <c r="E91" s="5" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" s="8" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
@@ -16491,9 +16496,9 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:6">
       <c r="A93" s="8" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
@@ -16502,9 +16507,9 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:6">
       <c r="A94" s="8" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
@@ -16513,9 +16518,9 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:6">
       <c r="A95" s="8" t="s">
-        <v>502</v>
+        <v>822</v>
       </c>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
@@ -16524,953 +16529,949 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:6">
       <c r="A96" s="8" t="s">
-        <v>317</v>
+        <v>502</v>
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
       <c r="E96" s="5" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="81">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" s="8" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="5" t="s">
-        <v>495</v>
-      </c>
+      <c r="D97" s="8"/>
       <c r="E97" s="5" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="81">
       <c r="A98" s="8" t="s">
-        <v>502</v>
+        <v>323</v>
       </c>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="5"/>
+      <c r="D98" s="5" t="s">
+        <v>495</v>
+      </c>
       <c r="E98" s="5" t="s">
-        <v>503</v>
+        <v>847</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="8" t="s">
-        <v>315</v>
+        <v>502</v>
       </c>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
+      <c r="D99" s="5"/>
       <c r="E99" s="5" t="s">
-        <v>1106</v>
+        <v>503</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
       <c r="E100" s="5" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="30">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" s="8" t="s">
-        <v>828</v>
+        <v>316</v>
       </c>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
       <c r="E101" s="5" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="45">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="30">
       <c r="A102" s="8" t="s">
-        <v>305</v>
+        <v>828</v>
       </c>
       <c r="B102" s="8"/>
-      <c r="C102" s="8" t="s">
-        <v>1259</v>
-      </c>
+      <c r="C102" s="8"/>
       <c r="D102" s="8"/>
       <c r="E102" s="5" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="30">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="45">
       <c r="A103" s="8" t="s">
-        <v>829</v>
+        <v>305</v>
       </c>
       <c r="B103" s="8"/>
-      <c r="C103" s="8"/>
+      <c r="C103" s="8" t="s">
+        <v>1259</v>
+      </c>
       <c r="D103" s="8"/>
       <c r="E103" s="5" t="s">
-        <v>1109</v>
+        <v>306</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="30">
       <c r="A104" s="8" t="s">
-        <v>310</v>
+        <v>829</v>
       </c>
       <c r="B104" s="8"/>
-      <c r="C104" s="8" t="s">
-        <v>1260</v>
-      </c>
+      <c r="C104" s="8"/>
       <c r="D104" s="8"/>
       <c r="E104" s="5" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="30">
       <c r="A105" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
+      <c r="C105" s="8" t="s">
+        <v>1260</v>
+      </c>
       <c r="D105" s="8"/>
       <c r="E105" s="5" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="30">
       <c r="A106" s="8" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
       <c r="E106" s="5" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="30">
       <c r="A107" s="8" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B107" s="8"/>
-      <c r="C107" s="8" t="s">
-        <v>1261</v>
-      </c>
+      <c r="C107" s="8"/>
       <c r="D107" s="8"/>
       <c r="E107" s="5" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8" t="s">
-        <v>830</v>
+        <v>321</v>
       </c>
       <c r="B108" s="8"/>
-      <c r="C108" s="8"/>
+      <c r="C108" s="8" t="s">
+        <v>1261</v>
+      </c>
       <c r="D108" s="8"/>
       <c r="E108" s="5" t="s">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="30">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="8" t="s">
-        <v>329</v>
+        <v>830</v>
       </c>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
       <c r="E109" s="5" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="30">
       <c r="A110" s="8" t="s">
-        <v>831</v>
+        <v>329</v>
       </c>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
       <c r="E110" s="5" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="30">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" s="8" t="s">
-        <v>332</v>
+        <v>831</v>
       </c>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
       <c r="E111" s="5" t="s">
-        <v>1114</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="30">
       <c r="A112" s="8" t="s">
-        <v>832</v>
+        <v>332</v>
       </c>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
       <c r="E112" s="5" t="s">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="30">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="8" t="s">
-        <v>337</v>
+        <v>832</v>
       </c>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
       <c r="E113" s="5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" s="6" customFormat="1">
-      <c r="A114" s="5" t="s">
-        <v>509</v>
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="30">
+      <c r="A114" s="8" t="s">
+        <v>337</v>
       </c>
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
-      <c r="D114" s="8" t="s">
-        <v>513</v>
-      </c>
+      <c r="D114" s="8"/>
       <c r="E114" s="5" t="s">
-        <v>512</v>
+        <v>338</v>
       </c>
     </row>
     <row r="115" spans="1:5" s="6" customFormat="1">
       <c r="A115" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="6" customFormat="1">
       <c r="A116" s="5" t="s">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>1116</v>
+        <v>511</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="5" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="5" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="5" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="5" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="5" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="5" t="s">
-        <v>590</v>
+        <v>517</v>
       </c>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8" t="s">
-        <v>591</v>
+        <v>519</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>678</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="5" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="5" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>713</v>
+        <v>679</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="5" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>680</v>
+        <v>713</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="5" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="5" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="5" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="5" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="5" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="5" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="5" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="5" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="5" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8" t="s">
-        <v>592</v>
+        <v>608</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="5" t="s">
-        <v>621</v>
+        <v>578</v>
       </c>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8" t="s">
-        <v>627</v>
+        <v>597</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E141" s="5" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E145" s="5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="5" t="s">
-        <v>648</v>
+        <v>626</v>
       </c>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8" t="s">
-        <v>654</v>
+        <v>632</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="5" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="E147" s="5" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="5" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="5" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E149" s="5" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="5" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="5" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E151" s="5" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="5" t="s">
-        <v>666</v>
+        <v>650</v>
       </c>
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8" t="s">
-        <v>672</v>
+        <v>658</v>
       </c>
       <c r="E152" s="5" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="5" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
       <c r="D153" s="8" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E153" s="5" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="5" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
       <c r="D154" s="8" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E154" s="5" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="5" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
       <c r="D155" s="8" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="5" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E156" s="5" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
       <c r="D157" s="8" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E157" s="5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="5" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
-      <c r="D158" s="5" t="s">
-        <v>733</v>
+      <c r="D158" s="8" t="s">
+        <v>677</v>
       </c>
       <c r="E158" s="5" t="s">
-        <v>1122</v>
+        <v>712</v>
       </c>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
       <c r="D159" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E159" s="5" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="5" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
       <c r="D160" s="5" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E160" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="5" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
-      <c r="D161" s="8" t="s">
-        <v>728</v>
+      <c r="D161" s="5" t="s">
+        <v>735</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
       <c r="D162" s="8" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E162" s="5" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="5" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
       <c r="D163" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
       <c r="D164" s="8" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="5" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
       <c r="D165" s="8" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E165" s="5" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="5" t="s">
-        <v>744</v>
+        <v>727</v>
       </c>
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
-      <c r="D166" s="5" t="s">
-        <v>748</v>
+      <c r="D166" s="8" t="s">
+        <v>732</v>
       </c>
       <c r="E166" s="5" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
       <c r="D167" s="5" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E167" s="5" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
       <c r="D168" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E168" s="5" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="5" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
       <c r="D169" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="E169" s="5" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="B170" s="8"/>
+      <c r="C170" s="8"/>
+      <c r="D170" s="5" t="s">
         <v>751</v>
       </c>
-      <c r="E169" s="5" t="s">
+      <c r="E170" s="5" t="s">
         <v>1133</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" ht="45">
-      <c r="A170" s="5" t="s">
-        <v>754</v>
-      </c>
-      <c r="B170" s="8">
-        <v>1</v>
-      </c>
-      <c r="C170" s="8"/>
-      <c r="D170" s="8" t="s">
-        <v>779</v>
-      </c>
-      <c r="E170" s="5" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="45">
@@ -17478,14 +17479,14 @@
         <v>754</v>
       </c>
       <c r="B171" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C171" s="8"/>
       <c r="D171" s="8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E171" s="5" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="45">
@@ -17493,214 +17494,231 @@
         <v>754</v>
       </c>
       <c r="B172" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="8" t="s">
+        <v>780</v>
+      </c>
+      <c r="E172" s="5" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" ht="45">
+      <c r="A173" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="B173" s="8">
+        <v>3</v>
+      </c>
+      <c r="C173" s="8"/>
+      <c r="D173" s="8" t="s">
         <v>781</v>
       </c>
-      <c r="E172" s="5" t="s">
+      <c r="E173" s="5" t="s">
         <v>1136</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="195">
-      <c r="A173" s="5" t="s">
+    <row r="174" spans="1:5" ht="195">
+      <c r="A174" s="5" t="s">
         <v>782</v>
-      </c>
-      <c r="B173" s="8"/>
-      <c r="C173" s="8" t="s">
-        <v>838</v>
-      </c>
-      <c r="D173" s="8"/>
-      <c r="E173" s="5" t="s">
-        <v>1137</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" ht="30">
-      <c r="A174" s="5" t="s">
-        <v>787</v>
       </c>
       <c r="B174" s="8"/>
       <c r="C174" s="8" t="s">
-        <v>788</v>
+        <v>838</v>
       </c>
       <c r="D174" s="8"/>
       <c r="E174" s="5" t="s">
-        <v>1166</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="30">
       <c r="A175" s="5" t="s">
-        <v>756</v>
+        <v>787</v>
       </c>
       <c r="B175" s="8"/>
       <c r="C175" s="8" t="s">
-        <v>1262</v>
+        <v>788</v>
       </c>
       <c r="D175" s="8"/>
       <c r="E175" s="5" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="30">
+      <c r="A176" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="B176" s="8"/>
+      <c r="C176" s="8" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D176" s="8"/>
+      <c r="E176" s="5" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="75">
-      <c r="A176" s="5" t="s">
+    <row r="177" spans="1:5" ht="75">
+      <c r="A177" s="5" t="s">
         <v>758</v>
-      </c>
-      <c r="B176" s="8"/>
-      <c r="C176" s="8"/>
-      <c r="D176" s="5" t="s">
-        <v>779</v>
-      </c>
-      <c r="E176" s="5" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" ht="30">
-      <c r="A177" s="5" t="s">
-        <v>760</v>
       </c>
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
-      <c r="D177" s="8"/>
+      <c r="D177" s="5" t="s">
+        <v>779</v>
+      </c>
       <c r="E177" s="5" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="30">
       <c r="A178" s="5" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
-      <c r="D178" s="8"/>
+      <c r="D178" s="8" t="s">
+        <v>783</v>
+      </c>
       <c r="E178" s="5" t="s">
-        <v>1138</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" ht="30">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
       <c r="A179" s="5" t="s">
-        <v>784</v>
+        <v>763</v>
       </c>
       <c r="B179" s="8"/>
-      <c r="C179" s="8" t="s">
-        <v>833</v>
-      </c>
+      <c r="C179" s="8"/>
       <c r="D179" s="8"/>
       <c r="E179" s="5" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="30">
       <c r="A180" s="5" t="s">
-        <v>765</v>
+        <v>784</v>
       </c>
       <c r="B180" s="8"/>
-      <c r="C180" s="8"/>
+      <c r="C180" s="8" t="s">
+        <v>833</v>
+      </c>
       <c r="D180" s="8"/>
       <c r="E180" s="5" t="s">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" ht="75">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
       <c r="A181" s="5" t="s">
-        <v>785</v>
+        <v>765</v>
       </c>
       <c r="B181" s="8"/>
-      <c r="C181" s="8" t="s">
-        <v>835</v>
-      </c>
+      <c r="C181" s="8"/>
       <c r="D181" s="8"/>
       <c r="E181" s="5" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" ht="20.25" customHeight="1">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="75">
       <c r="A182" s="5" t="s">
-        <v>767</v>
+        <v>785</v>
       </c>
       <c r="B182" s="8"/>
-      <c r="C182" s="8"/>
+      <c r="C182" s="8" t="s">
+        <v>835</v>
+      </c>
       <c r="D182" s="8"/>
       <c r="E182" s="5" t="s">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" ht="45">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="20.25" customHeight="1">
       <c r="A183" s="5" t="s">
-        <v>786</v>
+        <v>767</v>
       </c>
       <c r="B183" s="8"/>
-      <c r="C183" s="8" t="s">
-        <v>836</v>
-      </c>
+      <c r="C183" s="8"/>
       <c r="D183" s="8"/>
       <c r="E183" s="5" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" s="17" customFormat="1">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="45">
       <c r="A184" s="5" t="s">
-        <v>772</v>
+        <v>786</v>
       </c>
       <c r="B184" s="8"/>
-      <c r="C184" s="8"/>
+      <c r="C184" s="8" t="s">
+        <v>836</v>
+      </c>
       <c r="D184" s="8"/>
       <c r="E184" s="5" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" s="17" customFormat="1">
       <c r="A185" s="5" t="s">
-        <v>823</v>
+        <v>772</v>
       </c>
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
       <c r="D185" s="8"/>
       <c r="E185" s="5" t="s">
-        <v>1167</v>
+        <v>770</v>
       </c>
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="5" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B186" s="8"/>
       <c r="C186" s="8"/>
       <c r="D186" s="8"/>
       <c r="E186" s="5" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="5" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
       <c r="D187" s="8"/>
       <c r="E187" s="5" t="s">
-        <v>1142</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="5" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
       <c r="D188" s="8"/>
       <c r="E188" s="5" t="s">
-        <v>1168</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="5" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
       <c r="D189" s="8"/>
       <c r="E189" s="5" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="B190" s="8"/>
+      <c r="C190" s="8"/>
+      <c r="D190" s="8"/>
+      <c r="E190" s="5" t="s">
         <v>1167</v>
       </c>
     </row>
@@ -20298,7 +20316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099B6858-2052-4C2F-91E5-028849CAB7F9}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
suppress Sources - fix duplicate labels on master concept schema
</commit_message>
<xml_diff>
--- a/ISO19157-3/ISO19157-3_DQM.xlsx
+++ b/ISO19157-3/ISO19157-3_DQM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\ogc\iso1957-3-dqm-register\ISO19157-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E883CF-55E9-48BE-848B-F35B1E4F77BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4811C3A0-BC87-433C-8DA9-64A3AA1D15BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1020" windowWidth="27150" windowHeight="13995" tabRatio="712" activeTab="4" xr2:uid="{07ECC0CD-EFD9-442B-A5D4-A97E92D71BA8}"/>
+    <workbookView xWindow="960" yWindow="1020" windowWidth="27150" windowHeight="13995" tabRatio="712" activeTab="7" xr2:uid="{07ECC0CD-EFD9-442B-A5D4-A97E92D71BA8}"/>
   </bookViews>
   <sheets>
     <sheet name="URI" sheetId="9" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="1267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="1269">
   <si>
     <t>number of duplicate feature instances</t>
   </si>
@@ -7760,6 +7760,12 @@
   </si>
   <si>
     <t>FT28_4</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Reference Sources</t>
   </si>
 </sst>
 </file>
@@ -8534,14 +8540,14 @@
       </c>
       <c r="O2" s="27">
         <f t="shared" ref="O2:O33" ca="1" si="0">NOW()</f>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q2" s="27">
         <f t="shared" ref="Q2:Q65" ca="1" si="1">NOW()</f>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="2" customFormat="1" ht="30">
@@ -8589,14 +8595,14 @@
       </c>
       <c r="O3" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q3" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="2" customFormat="1" ht="45">
@@ -8644,14 +8650,14 @@
       </c>
       <c r="O4" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q4" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="178.5" customHeight="1">
@@ -8699,14 +8705,14 @@
       </c>
       <c r="O5" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q5" s="27">
         <f ca="1">NOW()</f>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="1" customFormat="1" ht="30">
@@ -8754,14 +8760,14 @@
       </c>
       <c r="O6" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q6" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="1" customFormat="1" ht="12.75" customHeight="1">
@@ -8809,14 +8815,14 @@
       </c>
       <c r="O7" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q7" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="46.5" customHeight="1">
@@ -8864,14 +8870,14 @@
       </c>
       <c r="O8" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q8" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="1" customFormat="1" ht="33.6" customHeight="1">
@@ -8919,14 +8925,14 @@
       </c>
       <c r="O9" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q9" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="1" customFormat="1" ht="33.6" customHeight="1">
@@ -8974,14 +8980,14 @@
       </c>
       <c r="O10" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q10" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="1" customFormat="1" ht="45.75" customHeight="1">
@@ -9029,12 +9035,12 @@
       </c>
       <c r="O11" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9082,14 +9088,14 @@
       </c>
       <c r="O12" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q12" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9137,14 +9143,14 @@
       </c>
       <c r="O13" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="Q13" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9192,14 +9198,14 @@
       </c>
       <c r="O14" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q14" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9247,14 +9253,14 @@
       </c>
       <c r="O15" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q15" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9298,14 +9304,14 @@
       </c>
       <c r="O16" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q16" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9353,14 +9359,14 @@
       </c>
       <c r="O17" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q17" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9408,14 +9414,14 @@
       </c>
       <c r="O18" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q18" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="19" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9463,14 +9469,14 @@
       </c>
       <c r="O19" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q19" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="20" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9518,14 +9524,14 @@
       </c>
       <c r="O20" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q20" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="21" spans="1:17" s="1" customFormat="1" ht="60">
@@ -9573,14 +9579,14 @@
       </c>
       <c r="O21" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q21" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="22" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9628,14 +9634,14 @@
       </c>
       <c r="O22" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q22" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="23" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9683,14 +9689,14 @@
       </c>
       <c r="O23" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q23" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="24" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9738,14 +9744,14 @@
       </c>
       <c r="O24" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q24" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="25" spans="1:17" s="1" customFormat="1" ht="45">
@@ -9793,14 +9799,14 @@
       </c>
       <c r="O25" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P25" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q25" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="26" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9848,14 +9854,14 @@
       </c>
       <c r="O26" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P26" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q26" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="27" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9903,14 +9909,14 @@
       </c>
       <c r="O27" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P27" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q27" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="28" spans="1:17" s="1" customFormat="1" ht="30">
@@ -9958,14 +9964,14 @@
       </c>
       <c r="O28" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P28" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q28" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="29" spans="1:17" s="1" customFormat="1" ht="90">
@@ -10005,14 +10011,14 @@
       </c>
       <c r="O29" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P29" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q29" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="30" spans="1:17" s="1" customFormat="1" ht="90">
@@ -10060,14 +10066,14 @@
       </c>
       <c r="O30" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P30" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q30" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="31" spans="1:17" s="5" customFormat="1" ht="90">
@@ -10115,14 +10121,14 @@
       </c>
       <c r="O31" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P31" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q31" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="32" spans="1:17" s="1" customFormat="1" ht="120">
@@ -10170,14 +10176,14 @@
       </c>
       <c r="O32" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P32" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q32" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="33" spans="1:17" s="1" customFormat="1" ht="60">
@@ -10225,14 +10231,14 @@
       </c>
       <c r="O33" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P33" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q33" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="34" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10280,14 +10286,14 @@
       </c>
       <c r="O34" s="27">
         <f t="shared" ref="O34:O65" ca="1" si="2">NOW()</f>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P34" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q34" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10335,14 +10341,14 @@
       </c>
       <c r="O35" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P35" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q35" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="36" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10390,14 +10396,14 @@
       </c>
       <c r="O36" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P36" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q36" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10445,14 +10451,14 @@
       </c>
       <c r="O37" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P37" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q37" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10500,14 +10506,14 @@
       </c>
       <c r="O38" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P38" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q38" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10553,14 +10559,14 @@
       </c>
       <c r="O39" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P39" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q39" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="40" spans="1:17" s="1" customFormat="1" ht="30">
@@ -10608,14 +10614,14 @@
       </c>
       <c r="O40" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P40" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q40" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="41" spans="1:17" s="1" customFormat="1" ht="75">
@@ -10663,14 +10669,14 @@
       </c>
       <c r="O41" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P41" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q41" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="5" customFormat="1" ht="75">
@@ -10715,14 +10721,14 @@
       </c>
       <c r="O42" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P42" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q42" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="43" spans="1:17" s="1" customFormat="1" ht="105">
@@ -10770,14 +10776,14 @@
       </c>
       <c r="O43" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q43" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="44" spans="1:17" s="1" customFormat="1" ht="45">
@@ -10825,14 +10831,14 @@
       </c>
       <c r="O44" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P44" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q44" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="45" spans="1:17" s="1" customFormat="1" ht="75">
@@ -10880,14 +10886,14 @@
       </c>
       <c r="O45" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P45" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q45" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="46" spans="1:17" s="1" customFormat="1" ht="45">
@@ -10935,14 +10941,14 @@
       </c>
       <c r="O46" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P46" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q46" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="47" spans="1:17" s="1" customFormat="1" ht="45">
@@ -10990,14 +10996,14 @@
       </c>
       <c r="O47" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q47" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="48" spans="1:17" s="1" customFormat="1" ht="30">
@@ -11045,14 +11051,14 @@
       </c>
       <c r="O48" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q48" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="49" spans="1:17" s="5" customFormat="1" ht="60">
@@ -11100,14 +11106,14 @@
       </c>
       <c r="O49" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q49" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="50" spans="1:17" s="1" customFormat="1" ht="60">
@@ -11153,14 +11159,14 @@
       </c>
       <c r="O50" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q50" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="51" spans="1:17" s="5" customFormat="1" ht="60">
@@ -11208,14 +11214,14 @@
       </c>
       <c r="O51" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P51" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q51" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="52" spans="1:17" s="5" customFormat="1" ht="60">
@@ -11263,14 +11269,14 @@
       </c>
       <c r="O52" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q52" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="53" spans="1:17" s="1" customFormat="1" ht="90">
@@ -11318,14 +11324,14 @@
       </c>
       <c r="O53" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q53" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="54" spans="1:17" s="1" customFormat="1" ht="60">
@@ -11373,14 +11379,14 @@
       </c>
       <c r="O54" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q54" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="55" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11428,14 +11434,14 @@
       </c>
       <c r="O55" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q55" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="56" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11483,14 +11489,14 @@
       </c>
       <c r="O56" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P56" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q56" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="57" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11538,14 +11544,14 @@
       </c>
       <c r="O57" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P57" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q57" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="58" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11593,14 +11599,14 @@
       </c>
       <c r="O58" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P58" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q58" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="59" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11648,14 +11654,14 @@
       </c>
       <c r="O59" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P59" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q59" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="60" spans="1:17" s="1" customFormat="1" ht="105">
@@ -11703,14 +11709,14 @@
       </c>
       <c r="O60" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P60" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q60" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="61" spans="1:17" s="1" customFormat="1" ht="30">
@@ -11758,14 +11764,14 @@
       </c>
       <c r="O61" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P61" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q61" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="1" customFormat="1" ht="45">
@@ -11813,14 +11819,14 @@
       </c>
       <c r="O62" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P62" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q62" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="63" spans="1:17" s="1" customFormat="1" ht="30">
@@ -11866,14 +11872,14 @@
       </c>
       <c r="O63" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P63" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q63" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="64" spans="1:17" s="1" customFormat="1" ht="45">
@@ -11921,14 +11927,14 @@
       </c>
       <c r="O64" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P64" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q64" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="65" spans="1:17" s="5" customFormat="1" ht="45">
@@ -11976,11 +11982,11 @@
       </c>
       <c r="O65" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="Q65" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="66" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12028,14 +12034,14 @@
       </c>
       <c r="O66" s="27">
         <f t="shared" ref="O66:O95" ca="1" si="3">NOW()</f>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P66" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q66" s="27">
         <f t="shared" ref="Q66:Q95" ca="1" si="4">NOW()</f>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="67" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12083,14 +12089,14 @@
       </c>
       <c r="O67" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P67" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q67" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="68" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12138,14 +12144,14 @@
       </c>
       <c r="O68" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q68" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12193,14 +12199,14 @@
       </c>
       <c r="O69" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q69" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12248,14 +12254,14 @@
       </c>
       <c r="O70" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q70" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="71" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12303,14 +12309,14 @@
       </c>
       <c r="O71" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q71" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="72" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12358,14 +12364,14 @@
       </c>
       <c r="O72" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q72" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12413,14 +12419,14 @@
       </c>
       <c r="O73" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q73" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="1" customFormat="1" ht="105">
@@ -12468,14 +12474,14 @@
       </c>
       <c r="O74" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P74" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q74" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12523,14 +12529,14 @@
       </c>
       <c r="O75" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P75" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q75" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="76" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12578,14 +12584,14 @@
       </c>
       <c r="O76" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P76" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q76" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="77" spans="1:17" s="1" customFormat="1" ht="45">
@@ -12633,14 +12639,14 @@
       </c>
       <c r="O77" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P77" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q77" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="78" spans="1:17" s="1" customFormat="1" ht="75">
@@ -12688,14 +12694,14 @@
       </c>
       <c r="O78" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P78" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q78" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="79" spans="1:17" s="1" customFormat="1" ht="75">
@@ -12743,14 +12749,14 @@
       </c>
       <c r="O79" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P79" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q79" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="30">
@@ -12798,14 +12804,14 @@
       </c>
       <c r="O80" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P80" s="5" t="s">
         <v>19</v>
       </c>
       <c r="Q80" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="75">
@@ -12853,14 +12859,14 @@
       </c>
       <c r="O81" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P81" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q81" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="30">
@@ -12908,14 +12914,14 @@
       </c>
       <c r="O82" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P82" s="5" t="s">
         <v>5</v>
       </c>
       <c r="Q82" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="60">
@@ -12959,14 +12965,14 @@
       </c>
       <c r="O83" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P83" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q83" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="84" spans="1:17" ht="45">
@@ -13014,14 +13020,14 @@
       </c>
       <c r="O84" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P84" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q84" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="45">
@@ -13069,14 +13075,14 @@
       </c>
       <c r="O85" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P85" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q85" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="86" spans="1:17" ht="60">
@@ -13124,14 +13130,14 @@
       </c>
       <c r="O86" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P86" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q86" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="60">
@@ -13179,14 +13185,14 @@
       </c>
       <c r="O87" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P87" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q87" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="30">
@@ -13234,14 +13240,14 @@
       </c>
       <c r="O88" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P88" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q88" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="89" spans="1:17" ht="30">
@@ -13289,14 +13295,14 @@
       </c>
       <c r="O89" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P89" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q89" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="90" spans="1:17" ht="30">
@@ -13344,14 +13350,14 @@
       </c>
       <c r="O90" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P90" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q90" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="30">
@@ -13399,14 +13405,14 @@
       </c>
       <c r="O91" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q91" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="92" spans="1:17" ht="45">
@@ -13452,14 +13458,14 @@
       </c>
       <c r="O92" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q92" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="30">
@@ -13507,14 +13513,14 @@
       </c>
       <c r="O93" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P93" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q93" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="45">
@@ -13558,14 +13564,14 @@
       </c>
       <c r="O94" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P94" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q94" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="30">
@@ -13611,14 +13617,14 @@
       </c>
       <c r="O95" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
       <c r="P95" s="5" t="s">
         <v>752</v>
       </c>
       <c r="Q95" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>45561.47881458333</v>
+        <v>45561.493416087964</v>
       </c>
     </row>
   </sheetData>
@@ -15335,7 +15341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C66609-5758-4067-9188-E18112A71DFE}">
   <dimension ref="A1:F190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B15" sqref="B15"/>
       <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
@@ -20314,10 +20320,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099B6858-2052-4C2F-91E5-028849CAB7F9}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20398,6 +20404,14 @@
         <v>1265</v>
       </c>
     </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1268</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>